<commit_message>
Restarted local git repo to get rid of Generation_Profiles.xlsx commit
</commit_message>
<xml_diff>
--- a/Google Maps/Generation_Geocode.xlsx
+++ b/Google Maps/Generation_Geocode.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uoa-student2\Desktop\Felipe Goncalves\Forschungscampus_Flexible_Elektrische_Netze_FEN\Google Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B089617B-E6F5-47A1-B488-34983A033460}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BC809E52-C08C-48DC-8640-EA98F7A9BD02}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8725" uniqueCount="3159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8726" uniqueCount="3160">
   <si>
     <t>Lfd. Nr.</t>
   </si>
@@ -9497,13 +9497,16 @@
   </si>
   <si>
     <t>WIN</t>
+  </si>
+  <si>
+    <t>I had to manually insert geodata, because Google Maps didn't have the given address</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9515,6 +9518,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9555,7 +9565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -9563,6 +9573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -9901,10 +9912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2120"/>
+  <dimension ref="A1:K2120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="C328" workbookViewId="0">
+      <selection activeCell="H333" sqref="H333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20161,7 +20172,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>321</v>
       </c>
@@ -20193,7 +20204,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>322</v>
       </c>
@@ -20225,7 +20236,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>323</v>
       </c>
@@ -20257,7 +20268,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>324</v>
       </c>
@@ -20289,7 +20300,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>325</v>
       </c>
@@ -20321,7 +20332,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>326</v>
       </c>
@@ -20353,7 +20364,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>327</v>
       </c>
@@ -20385,7 +20396,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>328</v>
       </c>
@@ -20417,7 +20428,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>329</v>
       </c>
@@ -20449,7 +20460,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>330</v>
       </c>
@@ -20481,7 +20492,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>331</v>
       </c>
@@ -20513,7 +20524,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>332</v>
       </c>
@@ -20545,7 +20556,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>333</v>
       </c>
@@ -20565,10 +20576,10 @@
         <v>45</v>
       </c>
       <c r="G333">
-        <v>50.913611199999998</v>
+        <v>50.741551000000001</v>
       </c>
       <c r="H333">
-        <v>6.7131178</v>
+        <v>6.1476829999999998</v>
       </c>
       <c r="I333">
         <v>30</v>
@@ -20576,8 +20587,11 @@
       <c r="J333" t="s">
         <v>3155</v>
       </c>
-    </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K333" s="3" t="s">
+        <v>3159</v>
+      </c>
+    </row>
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>334</v>
       </c>
@@ -20609,7 +20623,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>335</v>
       </c>
@@ -20641,7 +20655,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>336</v>
       </c>
@@ -77763,5 +77777,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created Load and Generator profiles
</commit_message>
<xml_diff>
--- a/Google Maps/Generation_Geocode.xlsx
+++ b/Google Maps/Generation_Geocode.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uoa-student2\Desktop\Felipe Goncalves\Forschungscampus_Flexible_Elektrische_Netze_FEN\Google Maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uoa-student2\Desktop\Felipe Goncalves\FlAixEnergy-Project\Google Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BC809E52-C08C-48DC-8640-EA98F7A9BD02}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9083D043-1E27-4605-AB2B-701DE842C32A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9914,8 +9914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C328" workbookViewId="0">
-      <selection activeCell="H333" sqref="H333"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U535" sqref="U535"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>